<commit_message>
got rid of 'shopt' error
</commit_message>
<xml_diff>
--- a/example_testfile.xlsx
+++ b/example_testfile.xlsx
@@ -2,23 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="5430" windowWidth="17268" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
   <si>
     <t>IP</t>
   </si>
@@ -38,9 +35,6 @@
     <t>103.44.63.75</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>104.131.161.182</t>
   </si>
   <si>
@@ -378,43 +372,20 @@
   </si>
   <si>
     <t>94.73.149.51</t>
-  </si>
-  <si>
-    <t>{"undetected_urls": [], "undetected_downloaded_samples": [{"date": "2017-10-26 07:54:01", "positives": 0, "total": 69, "sha256": "0755216afc1f8efebd0882e43ad84f41fcc5cd22ccd6dc9ac81ff88997c43427"}, {"date": "2018-06-20 19:16:49", "positives": 0, "total": 0, "sha256": "0e99c26de560c4ec633ca9287d3a92a08bc16bce0b330f4d7f2f31d28cc8fa02"}, {"date": "2018-06-20 17:18:01", "positives": 0, "total": 0, "sha256": "dc745bbef34c494c1344502aaa66f349097615abb0ec2748f1944673833bd22c"}, {"date": "2018-06-14 19:49:16", "positives": 0, "total": 0, "sha256": "4a06ab206c89a74a5169a74cdf615a72746d9271bc4b8f7dc0976d98c2737aaa"}, {"date": "2016-04-25 14:20:44", "positives": 0, "total": 57, "sha256": "9dd8a4209bbce6a42c79a872364859acd8ffbab5fc5b9bcbf39b10f3e05aae7b"}, {"date": "2018-04-20 09:50:19", "positives": 0, "total": 54, "sha256": "158c99d5bfd5ef2901f773eaed4dc561f45237bc7c130052fe026470fac30576"}, {"date": "2018-04-20 09:00:06", "positives": 0, "total": 61, "sha256": "7eaf81abfe11530842d8169cb2579af0784cd98e7f1d9eac2aca8192128f0eb8"}, {"date": "2018-03-27 16:58:23", "positives": 0, "total": 55, "sha256": "0b320ead9ab97632c612d0ff1532e8c0909b1299d3a5ab4894c8ff7933e84730"}, {"date": "2018-02-25 11:09:43", "positives": 0, "total": 58, "sha256": "b38a93e43e0f834284b51a981542bc8cdfc5fe016396fe83454d337f33ca71aa"}, {"date": "2018-02-03 10:09:24", "positives": 0, "total": 0, "sha256": "3c46aaeafac2f62859560824982cf8b6d5faaf230a1e65566feaebf45179831a"}, {"date": "2018-02-03 05:13:36", "positives": 0, "total": 56, "sha256": "98df35b97cf50c1e361300c18e19c924c1590a367d70bed97c0f0ac723be8a52"}, {"date": "2017-12-07 12:21:45", "positives": 0, "total": 58, "sha256": "f2319a304f1b162f190a0f3dedfd6222b003152a8b44e5ed8ff9f761473920f6"}, {"date": "2017-11-28 11:15:37", "positives": 0, "total": 0, "sha256": "0f115aaf1656b6c0fd92950ad33221c86fe7c3e2fb34c86dce909c19f4fc6fe2"}, {"date": "2017-10-29 16:18:07", "positives": 0, "total": 56, "sha256": "646fa67849355d331e9a37022f84a7296d647aabe7b6544b3bac955f06ba076c"}, {"date": "2017-10-19 14:29:18", "positives": 0, "total": 56, "sha256": "e39724115a471f75712213216021f98bc6688ea5400b0a930d32d5e9c595fd83"}, {"date": "2017-10-04 14:45:58", "positives": 0, "total": 60, "sha256": "32ac321b712f05735a19335a3414aee261c2e67d2325749a55217277715ad89d"}, {"date": "2017-09-24 09:32:33", "positives": 0, "total": 60, "sha256": "8731adc5ca1869cd535152b367a563b5e739fe87bb91e6dcc2955d871e83e646"}, {"date": "2017-09-08 12:47:52", "positives": 0, "total": 56, "sha256": "967b1d33e2d86af85d036154cccc6d62d6db2b7daae7ab154e46d0993ce9d77c"}, {"date": "2017-08-28 15:52:25", "positives": 0, "total": 55, "sha256": "4d03fa3a6837cb8348d20da84f3830c2362e37de5c9aff0f6ac7a2262a273486"}, {"date": "2017-08-27 11:07:24", "positives": 0, "total": 58, "sha256": "9ccaa611f0b77cc12c229252b021bb43b84ed593c83cfa9a8a39f0d045d18e52"}, {"date": "2017-08-21 09:06:48", "positives": 0, "total": 57, "sha256": "0022afec6602a8a02120035b6b48f62a6f479fd7f1ffdb7c98c05b1ffbec29c7"}, {"date": "2017-07-25 12:08:55", "positives": 0, "total": 0, "sha256": "c3e2135af12f5b893fbe2bf16e3d7303712d6036ae402901306676c9aa1caaa3"}, {"date": "2017-05-11 05:05:06", "positives": 0, "total": 55, "sha256": "e4595cbec16bb83c1203d601f96fb32c8f38951484ef5b4816329a3155137ba6"}, {"date": "2017-01-21 12:25:04", "positives": 0, "total": 0, "sha256": "40fc9569e6cc3b327cb772f0df6c8186f501ae7bba94a4fbc58df5ea6d679f0a"}, {"date": "2016-12-02 11:46:41", "positives": 0, "total": 57, "sha256": "1cbfc6a0a109c6209800cc83c6e23434306c4dcd22f3b17f5200440de482c557"}], "country": "ZZ", "response_code": 1, "verbose_msg": "IP address in dataset", "detected_downloaded_samples": [{"date": "2018-06-23 11:38:19", "positives": 30, "total": 67, "sha256": "48d337f331798f6818b9d1225bf95255f2a355ac4f48d39cec288731ecf5dd80"}, {"date": "2018-06-21 04:59:35", "positives": 17, "total": 60, "sha256": "6e2d27297793d1d94e000d3c377e3feca848b54a068b73915b33d806175b9e07"}, {"date": "2018-06-20 22:09:05", "positives": 16, "total": 60, "sha256": "9b01ac054e2434c393a0626a7e341175d312bb3dcf22c6f46c2702c15387fbd6"}, {"date": "2018-06-20 19:27:25", "positives": 16, "total": 60, "sha256": "0e99c26de560c4ec633ca9287d3a92a08bc16bce0b330f4d7f2f31d28cc8fa02"}, {"date": "2018-06-20 17:10:06", "positives": 16, "total": 58, "sha256": "ef9296574ae1f8fcea94d03867972f9c2cae555562415a3401c71a46b2a46f87"}, {"date": "2018-06-20 15:39:18", "positives": 17, "total": 59, "sha256": "f70d253b89d41d92211f95346b82cc475a5a518521e94a1a12d4ac0a9520d51a"}, {"date": "2018-06-20 14:27:37", "positives": 17, "total": 71, "sha256": "d5fa277192228171e711c082a39770c765e06e493d79fb6d42b7e9a2c001c1fd"}, {"date": "2018-06-18 08:24:25", "positives": 15, "total": 58, "sha256": "edc2ac668d69a2158f2f1015d10b7b03fbf00dbc1c7eae3342cdec295709dd7b"}, {"date": "2018-06-18 06:47:08", "positives": 14, "total": 59, "sha256": "7299ed9aa47dd731fd8176acf619278967ad7042cb12c2aefb49cfc9e2cd087a"}, {"date": "2018-06-15 04:10:57", "positives": 40, "total": 60, "sha256": "05bc07546bd2ec1236fff218c709fe919951d7376b33641a01dc47fcb0e7ba09"}, {"date": "2018-06-14 20:31:24", "positives": 16, "total": 71, "sha256": "48cc6fa1047e38a2a2f6f3ce6ff871839a356c10f3a0682b832946585e2d95f4"}, {"date": "2018-06-14 09:57:09", "positives": 18, "total": 59, "sha256": "9dc2a658ff65ada5b6e998322a3b9a173c6803302c4017ed797843dd8307e95e"}, {"date": "2018-06-12 02:39:07", "positives": 42, "total": 71, "sha256": "8df62bd5d06ce9bd70d1d58d57ec82b69dba692ce544cf14f615688b8d6f2b5f"}, {"date": "2018-06-08 04:20:47", "positives": 38, "total": 60, "sha256": "22b94903d6c21b6af7e3aec0e6e0799f49b3c7da9316aa68d6cb92c4ded80f62"}, {"date": "2018-05-31 16:49:06", "positives": 12, "total": 60, "sha256": "c7ef4f32f3f149b5b5fdc23bded5d171c8cd92b3fd2fc3ca3a85f99aba583f32"}, {"date": "2018-05-31 16:31:29", "positives": 12, "total": 60, "sha256": "4c5859d232fc7c0d9305d814a0c361d0dcbb8031db801adce92159ef8d03c691"}, {"date": "2018-05-31 13:09:55", "positives": 16, "total": 58, "sha256": "342a41215ef86857aee77f9716730e07b5f13fbcb84176ea690b6306c7651d1e"}, {"date": "2018-05-31 05:33:55", "positives": 13, "total": 60, "sha256": "563dd537196cfeee5560e51f7ee9b0fc067062cb5a3dfb2dc0a967f77b31bd99"}, {"date": "2018-05-30 22:22:27", "positives": 14, "total": 71, "sha256": "fe9736294556b6269116301f9e581bae4e231357d9b73c8122dd40df1e0a5a68"}, {"date": "2018-05-30 21:52:15", "positives": 19, "total": 59, "sha256": "253cb62fc1815ff5c87bb2182936d860c413ef358224f4d8a5d43a0223dc69f3"}, {"date": "2018-05-29 03:23:59", "positives": 12, "total": 60, "sha256": "b05b6c86a56621f042d00b967cadac2e088d9494cdac6c58e18a2977e8e05a5e"}, {"date": "2018-05-28 14:34:45", "positives": 11, "total": 60, "sha256": "2aff05778e075cf559a292cb002a9cdbe631d5f9f21d4d84be1216b80e4ff742"}, {"date": "2018-05-27 11:12:08", "positives": 28, "total": 60, "sha256": "b4fdb77c5b6eede55fa1025dcbd522ada24dc6fef82efbeac60934cb6a8e8005"}, {"date": "2018-05-24 09:14:43", "positives": 11, "total": 70, "sha256": "0c2a99e6c14c8916a9dee5219ea3b9afee8806cc92124b536f54eb4fbb4f72a9"}, {"date": "2018-05-23 19:43:49", "positives": 16, "total": 70, "sha256": "c669bf059a738dd4fbcb9311f85217987978d901ff7386aa6d4cf52f836aeb18"}, {"date": "2018-05-22 00:40:04", "positives": 8, "total": 70, "sha256": "c0729500d7f3863b2b9ccae42c838f68d97870583cd99e4981939c5a7ae04f55"}, {"date": "2018-05-16 23:42:03", "positives": 17, "total": 69, "sha256": "d4c4f3bbdc9ae9f6b61aef2dfad86fdb31a61d65cc482276776a148586c7a2ed"}, {"date": "2017-10-20 16:08:22", "positives": 52, "total": 66, "sha256": "e7def648f10c23a32125e7d663327c87b092f2aeb71c87af19a6c4c03828e7d8"}, {"date": "2017-10-13 11:45:44", "positives": 11, "total": 69, "sha256": "270d9d6d55ef94d5c42513f2a92cf64322a036ce5bbf696d69ead4b7c30813cb"}, {"date": "2017-10-12 20:23:59", "positives": 16, "total": 65, "sha256": "300fca0df694a74d08389e7d4963dcc2aa88b35761d5db60c0919d28cf11e98b"}, {"date": "2017-08-18 20:11:45", "positives": 16, "total": 60, "sha256": "cfbbfaaf0eb5c7735033e9f0fa569f6259b150af297f33f56b9716e624277458"}, {"date": "2017-07-27 04:08:22", "positives": 16, "total": 59, "sha256": "352fa1a99bd73894525c1b6c814d17c5329edd398ba15de8410fb2c5ac7b285d"}, {"date": "2017-07-26 06:20:55", "positives": 13, "total": 60, "sha256": "2db72da8c5aaf57e5417afd6b058a2b008798ff1378b65c4eb316ea95de0089e"}, {"date": "2017-06-29 12:57:45", "positives": 4, "total": 56, "sha256": "27e945d4c24b6588dbf46b9cefbc98215d8e98b42e9069dc672ec764d97a1ef1"}], "resolutions": [{"last_resolved": "2018-02-09 00:00:00", "hostname": "0.boa.hk"}, {"last_resolved": "2018-04-22 08:07:34", "hostname": "3-mart.com.hk"}, {"last_resolved": "2018-07-26 05:56:14", "hostname": "5d51.com"}, {"last_resolved": "2017-07-23 00:00:00", "hostname": "a.healthyme.com"}, {"last_resolved": "2018-04-21 08:50:39", "hostname": "accollege.net"}, {"last_resolved": "2018-07-04 01:37:41", "hostname": "actorsfamily.com.hk"}, {"last_resolved": "2018-04-30 04:25:54", "hostname": "adagencyasia.com.hk"}, {"last_resolved": "2016-12-08 00:00:00", "hostname": "americanclubs.org"}, {"last_resolved": "2018-07-26 08:09:09", "hostname": "amport-group.com"}, {"last_resolved": "2017-09-02 00:00:00", "hostname": "ancoele.com.hk"}, {"last_resolved": "2018-05-25 21:41:15", "hostname": "andrewmaknco.com.hk"}, {"last_resolved": "2018-05-17 15:47:57", "hostname": "angelbluebeauty.com.hk"}, {"last_resolved": "2018-07-26 19:10:22", "hostname": "angelini-hospitality.com"}, {"last_resolved": "2018-07-06 21:37:15", "hostname": "angelini-hotels.com"}, {"last_resolved": "2018-07-25 06:01:07", "hostname": "angelinihospitality.com"}, {"last_resolved": "2018-07-04 13:59:42", "hostname": "angelinihotels.com"}, {"last_resolved": "2016-10-12 00:00:00", "hostname": "anthonyblcheung.org"}, {"last_resolved": "2018-06-28 14:31:11", "hostname": "apexdesign.com.hk"}, {"last_resolved": "2018-03-29 00:00:00", "hostname": "arm.com.hk"}, {"last_resolved": "2018-06-29 21:40:11", "hostname": "artphoenix.com.hk"}, {"last_resolved": "2018-07-26 05:52:24", "hostname": "asia-packing.com"}, {"last_resolved": "2018-05-15 11:32:35", "hostname": "astglobalexpress.com"}, {"last_resolved": "2018-04-22 13:13:19", "hostname": "aworldtech.vizzhost.com"}, {"last_resolved": "2018-07-04 06:43:22", "hostname": "baby-lovers.com"}, {"last_resolved": "2018-07-26 14:57:20", "hostname": "bellatam.com"}, {"last_resolved": "2016-12-08 00:00:00", "hostname": "beltone-hearing.com.hk"}, {"last_resolved": "2018-07-26 06:00:16", "hostname": "big-collection.com"}, {"last_resolved": "2016-10-02 00:00:00", "hostname": "bioprobeshk.com"}, {"last_resolved": "2018-07-04 06:45:56", "hostname": "bnsconcord.com"}, {"last_resolved": "2018-06-30 08:38:13", "hostname": "boa.hk"}, {"last_resolved": "2018-07-24 20:07:14", "hostname": "bop.com.hk"}, {"last_resolved": "2018-06-23 15:08:25", "hostname": "bt-links.com.hk"}, {"last_resolved": "2018-06-09 21:57:06", "hostname": "buzanhk.com"}, {"last_resolved": "2018-04-25 21:33:09", "hostname": "catbus-adventures.com.hk"}, {"last_resolved": "2018-04-28 05:41:51", "hostname": "centralurology.com.hk"}, {"last_resolved": "2018-07-25 06:14:22", "hostname": "chant.com.hk"}, {"last_resolved": "2016-11-27 00:00:00", "hostname": "chartlyent.com"}, {"last_resolved": "2016-11-21 00:00:00", "hostname": "cheungon.vizzhost.com"}, {"last_resolved": "2018-07-20 21:38:16", "hostname": "chinaworldtravel.com.hk"}, {"last_resolved": "2016-12-10 00:00:00", "hostname": "chongkin.vizzhost.com"}, {"last_resolved": "2018-07-25 21:40:31", "hostname": "citipage.com.hk"}, {"last_resolved": "2018-07-26 18:38:58", "hostname": "ckskartracing.com.hk"}, {"last_resolved": "2018-07-26 02:36:42", "hostname": "conoilic.com"}, {"last_resolved": "2018-07-26 15:12:08", "hostname": "cplaromasfareast.com.hk"}, {"last_resolved": "2018-05-21 17:43:29", "hostname": "cs-consultancy.com"}, {"last_resolved": "2018-07-04 02:04:32", "hostname": "cwm-nethersole-fund.org.hk"}, {"last_resolved": "2018-07-24 14:27:11", "hostname": "deerhillbay.com.hk"}, {"last_resolved": "2018-07-03 09:04:13", "hostname": "deli-honour.com"}, {"last_resolved": "2017-04-15 00:00:00", "hostname": "dermanova.vizzhost.com"}, {"last_resolved": "2017-03-23 00:00:00", "hostname": "digitalonline.hk"}, {"last_resolved": "2016-09-30 00:00:00", "hostname": "diluxlighting.com"}, {"last_resolved": "2018-07-03 18:54:18", "hostname": "dsuccess.net"}, {"last_resolved": "2018-07-03 18:57:17", "hostname": "e-accounts.net"}, {"last_resolved": "2016-11-15 00:00:00", "hostname": "e-goodss.com"}, {"last_resolved": "2018-07-03 04:17:27", "hostname": "eaas.com.hk"}, {"last_resolved": "2018-07-03 17:27:30", "hostname": "ec-soccer.com"}, {"last_resolved": "2017-11-20 00:00:00", "hostname": "effer.com.cn"}, {"last_resolved": "2018-07-25 16:58:19", "hostname": "elastape.com"}, {"last_resolved": "2018-07-20 06:19:00", "hostname": "elekon.com.hk"}, {"last_resolved": "2018-07-10 19:54:51", "hostname": "entgulf.com"}, {"last_resolved": "2018-04-16 00:00:00", "hostname": "expert.com.hk"}, {"last_resolved": "2018-05-01 08:46:45", "hostname": "fastlane.hk"}, {"last_resolved": "2018-07-22 20:54:02", "hostname": "ferry.com.hk"}, {"last_resolved": "2018-06-10 07:39:39", "hostname": "forum.sharewithyou.com"}, {"last_resolved": "2018-07-26 07:06:28", "hostname": "ftl-hk.com"}, {"last_resolved": "2018-07-26 05:17:54", "hostname": "fubsypig.com"}, {"last_resolved": "2017-04-24 00:00:00", "hostname": "fufaikitchen.com"}, {"last_resolved": "2018-04-27 07:28:30", "hostname": "garesch.com"}, {"last_resolved": "2017-10-17 00:00:00", "hostname": "geegeejerjer.com"}, {"last_resolved": "2018-06-01 01:43:56", "hostname": "generaliasia.com.hk"}, {"last_resolved": "2018-07-18 03:03:22", "hostname": "globegloves.com.hk"}, {"last_resolved": "2018-05-16 21:45:52", "hostname": "goldenratio.hk"}, {"last_resolved": "2018-07-26 09:45:58", "hostname": "goldinhk.com"}, {"last_resolved": "2018-07-26 06:31:51", "hostname": "greatwellfood.com"}, {"last_resolved": "2018-04-29 10:38:08", "hostname": "hagerasia.com.hk"}, {"last_resolved": "2018-07-26 08:42:22", "hostname": "hangfuk.com"}, {"last_resolved": "2018-05-02 09:30:41", "hostname": "hangleei.com.hk"}, {"last_resolved": "2017-11-11 00:00:00", "hostname": "harboursun.vizzhost.com"}, {"last_resolved": "2018-07-24 18:18:28", "hostname": "harvest-trend.com.hk"}, {"last_resolved": "2018-07-26 20:53:48", "hostname": "healthyme.com"}, {"last_resolved": "2018-07-24 18:44:27", "hostname": "healthyme.com.hk"}, {"last_resolved": "2018-07-10 16:19:33", "hostname": "healthyme.hk"}, {"last_resolved": "2018-06-11 17:56:49", "hostname": "hkbcf.org.hk"}, {"last_resolved": "2018-07-26 06:02:04", "hostname": "hkjoyful.com"}, {"last_resolved": "2017-04-01 00:00:00", "hostname": "hungshing.vizzhost.com"}, {"last_resolved": "2018-04-23 13:19:05", "hostname": "ideng.com.hk"}, {"last_resolved": "2017-08-23 00:00:00", "hostname": "idlhk.com"}, {"last_resolved": "2018-07-25 20:16:59", "hostname": "implexsys.com"}, {"last_resolved": "2018-07-24 06:15:09", "hostname": "interconcept.com.hk"}, {"last_resolved": "2018-07-25 17:53:52", "hostname": "izserver.com"}, {"last_resolved": "2016-12-05 00:00:00", "hostname": "j-zip.com.hk"}, {"last_resolved": "2018-07-26 19:34:53", "hostname": "jackwah.com"}, {"last_resolved": "2018-07-25 02:55:59", "hostname": "jameswong.hk"}, {"last_resolved": "2018-07-25 06:56:22", "hostname": "jesterkitty.com"}, {"last_resolved": "2018-07-24 09:30:05", "hostname": "jungao.com.hk"}, {"last_resolved": "2018-07-25 14:57:39", "hostname": "k-lefevre.com"}, {"last_resolved": "2018-07-26 06:32:16", "hostname": "kbchk.com"}, {"last_resolved": "2017-11-02 00:00:00", "hostname": "kennybb.net"}, {"last_resolved": "2018-05-27 05:33:41", "hostname": "kimberly.com.hk"}, {"last_resolved": "2018-07-24 18:57:13", "hostname": "kittyjester.com"}, {"last_resolved": "2018-07-26 17:24:37", "hostname": "kmfal.com"}, {"last_resolved": "2018-07-04 10:54:32", "hostname": "kwan-tat.com"}, {"last_resolved": "2018-03-07 00:00:00", "hostname": "kwokming.com"}, {"last_resolved": "2018-07-17 12:51:59", "hostname": "lavorwash.com.hk"}, {"last_resolved": "2018-05-01 23:50:17", "hostname": "lawrencelam.idv.hk"}, {"last_resolved": "2018-07-04 05:12:28", "hostname": "legendtoys.com.hk"}, {"last_resolved": "2018-05-07 07:50:00", "hostname": "lichton.com.hk"}, {"last_resolved": "2018-04-19 01:37:14", "hostname": "linkongkee.com.hk"}, {"last_resolved": "2018-07-26 05:27:13", "hostname": "logicworkshop.com"}, {"last_resolved": "2016-12-31 00:00:00", "hostname": "loongka.com"}, {"last_resolved": "2017-05-07 00:00:00", "hostname": "mabelle.vizzhost.com"}, {"last_resolved": "2018-07-26 00:55:54", "hostname": "madcradleonline.com"}, {"last_resolved": "2018-07-11 17:14:13", "hostname": "mamannbebe.com"}, {"last_resolved": "2016-12-02 00:00:00", "hostname": "masterclean.hk"}, {"last_resolved": "2018-05-06 13:54:09", "hostname": "masterkids.com.hk"}, {"last_resolved": "2018-06-30 13:21:27", "hostname": "maxhomes.com.hk"}, {"last_resolved": "2018-07-25 21:19:33", "hostname": "medequip.com.hk"}, {"last_resolved": "2018-07-26 19:37:19", "hostname": "midashk.com"}, {"last_resolved": "2018-07-25 08:55:07", "hostname": "mindmapping.hk"}, {"last_resolved": "2018-07-03 14:44:24", "hostname": "monsterworkshop.com"}, {"last_resolved": "2017-02-02 00:00:00", "hostname": "mso.hk"}, {"last_resolved": "2018-04-27 09:05:09", "hostname": "nelsonandcompany.com.hk"}, {"last_resolved": "2018-07-26 20:08:03", "hostname": "nelsonchtam.com.hk"}, {"last_resolved": "2018-05-03 09:36:52", "hostname": "neptunegroup.com.hk"}, {"last_resolved": "2016-12-06 00:00:00", "hostname": "nethersole-ss-ucnh.org.hk"}, {"last_resolved": "2018-07-22 07:39:56", "hostname": "newsound.com.hk"}, {"last_resolved": "2018-04-27 14:11:53", "hostname": "nextstep.com.hk"}, {"last_resolved": "2016-12-01 00:00:00", "hostname": "nr-properties.com"}, {"last_resolved": "2018-07-04 00:39:11", "hostname": "ns1.izserver.com"}, {"last_resolved": "2018-07-25 17:53:26", "hostname": "ns2.izserver.com"}, {"last_resolved": "2018-05-07 20:05:42", "hostname": "nwpf.com.hk"}, {"last_resolved": "2017-04-28 00:00:00", "hostname": "oceangrace.com.hk"}, {"last_resolved": "2018-07-08 22:41:04", "hostname": "omnimax.com.hk"}, {"last_resolved": "2018-07-03 10:08:39", "hostname": "petegg.com"}, {"last_resolved": "2018-07-04 17:56:32", "hostname": "petztalk.com"}, {"last_resolved": "2018-06-11 09:50:00", "hostname": "pilotstar.com.hk"}, {"last_resolved": "2018-06-15 21:37:41", "hostname": "poly-tech.com.hk"}, {"last_resolved": "2018-04-26 02:16:30", "hostname": "premierland.com.hk"}, {"last_resolved": "2016-12-09 00:00:00", "hostname": "q-worklife21.com"}, {"last_resolved": "2018-07-26 07:45:24", "hostname": "raymondloo.net"}, {"last_resolved": "2016-10-01 00:00:00", "hostname": "redgoodss.com"}, {"last_resolved": "2018-05-19 13:19:15", "hostname": "regionfine.com.hk"}, {"last_resolved": "2018-07-17 19:51:19", "hostname": "richgoldman.com.hk"}, {"last_resolved": "2018-07-04 23:02:16", "hostname": "rogeryuen.com"}, {"last_resolved": "2017-06-29 00:00:00", "hostname": "roriktech.com"}, {"last_resolved": "2018-07-26 06:34:19", "hostname": "rwnt.com"}, {"last_resolved": "2018-07-25 02:53:37", "hostname": "rxezy.com"}, {"last_resolved": "2018-04-22 13:10:38", "hostname": "sakong.com.hk"}, {"last_resolved": "2018-07-25 15:46:02", "hostname": "senseswine.com"}, {"last_resolved": "2018-07-04 03:27:02", "hostname": "serviceprint1968.com"}, {"last_resolved": "2018-07-24 10:21:55", "hostname": "servoair.com.hk"}, {"last_resolved": "2018-07-25 02:58:13", "hostname": "sha-hk.com"}, {"last_resolved": "2018-07-26 09:18:40", "hostname": "sharewithyou.com"}, {"last_resolved": "2018-04-27 16:33:45", "hostname": "sharonhui.idv.hk"}, {"last_resolved": "2018-07-25 18:15:41", "hostname": "showsweets.com"}, {"last_resolved": "2016-11-28 00:00:00", "hostname": "succi.cn"}, {"last_resolved": "2016-11-28 00:00:00", "hostname": "succi.com.cn"}, {"last_resolved": "2016-12-25 00:00:00", "hostname": "summercommunication.com"}, {"last_resolved": "2017-03-09 00:00:00", "hostname": "summeriff.vizzhost.com"}, {"last_resolved": "2018-07-26 07:37:51", "hostname": "sunhingchurch.org"}, {"last_resolved": "2016-09-23 00:00:00", "hostname": "sunming.com.hk"}, {"last_resolved": "2018-07-05 01:42:32", "hostname": "thinking-up.com"}, {"last_resolved": "2018-07-03 17:57:27", "hostname": "timerichinvestment.com"}, {"last_resolved": "2018-07-26 18:34:07", "hostname": "tinyfilmunit.com"}, {"last_resolved": "2018-07-19 02:07:52", "hostname": "toki.com.hk"}, {"last_resolved": "2017-04-11 00:00:00", "hostname": "tpshc.org"}, {"last_resolved": "2018-07-26 15:13:01", "hostname": "trendgroup.com"}, {"last_resolved": "2018-07-25 00:48:39", "hostname": "tungyuen.net"}, {"last_resolved": "2018-06-02 21:42:01", "hostname": "twowings.com.hk"}, {"last_resolved": "2018-07-08 13:19:20", "hostname": "ultraformgroup.com.hk"}, {"last_resolved": "2017-08-31 00:00:00", "hostname": "vanjar.com"}, {"last_resolved": "2018-07-23 23:09:50", "hostname": "viewing.com.hk"}, {"last_resolved": "2018-07-25 17:51:15", "hostname": "viibiz.com"}, {"last_resolved": "2018-05-01 13:03:27", "hostname": "viipos.com"}, {"last_resolved": "2017-12-18 00:00:00", "hostname": "vingtsun-hk.com"}, {"last_resolved": "2018-07-03 00:59:27", "hostname": "vizz.hk"}, {"last_resolved": "2016-09-26 00:00:00", "hostname": "vizzgroup.com"}, {"last_resolved": "2018-05-15 04:54:30", "hostname": "vizzgroup.com.hk"}, {"last_resolved": "2018-07-26 18:58:01", "hostname": "vizzhosting.com"}, {"last_resolved": "2018-07-26 16:04:12", "hostname": "waddyjew.com"}, {"last_resolved": "2018-07-18 22:52:58", "hostname": "wai-ming.com.hk"}, {"last_resolved": "2016-09-19 00:00:00", "hostname": "waifungcontainer.com"}, {"last_resolved": "2017-09-01 00:00:00", "hostname": "waiminghong.com.hk"}, {"last_resolved": "2016-12-31 00:00:00", "hostname": "wcp.hkmcadventist.org"}, {"last_resolved": "2018-05-02 09:30:29", "hostname": "wcp.richburgmotors.com"}, {"last_resolved": "2018-02-10 00:00:00", "hostname": "wcp.salutemodels.com"}, {"last_resolved": "2016-11-26 00:00:00", "hostname": "wcp.vizzhost.com"}, {"last_resolved": "2016-12-13 00:00:00", "hostname": "weidner-cleaning.cn"}, {"last_resolved": "2016-12-13 00:00:00", "hostname": "weidner.cn"}, {"last_resolved": "2018-07-18 21:59:10", "hostname": "wellmax.com.hk"}, {"last_resolved": "2018-07-26 16:11:34", "hostname": "welmex.com"}, {"last_resolved": "2018-04-15 16:16:29", "hostname": "wheeler.com.hk"}, {"last_resolved": "2018-07-16 05:45:58", "hostname": "whittohodesign.com"}, {"last_resolved": "2018-07-26 09:26:44", "hostname": "winsino.com"}, {"last_resolved": "2018-07-04 06:19:39", "hostname": "wisegesl.com"}, {"last_resolved": "2018-07-03 13:12:02", "hostname": "wongtinyan.com"}, {"last_resolved": "2018-07-03 08:20:25", "hostname": "wpphk.com"}, {"last_resolved": "2016-10-20 00:00:00", "hostname": "www.24red.com.hk"}, {"last_resolved": "2018-04-22 08:07:33", "hostname": "www.3-mart.com.hk"}, {"last_resolved": "2018-04-21 08:50:39", "hostname": "www.accollege.net"}, {"last_resolved": "2018-05-25 23:54:28", "hostname": "www.actorsfamily.com.hk"}, {"last_resolved": "2018-04-30 04:25:52", "hostname": "www.adagencyasia.com.hk"}, {"last_resolved": "2017-02-03 00:00:00", "hostname": "www.ancoele.com.hk"}, {"last_resolved": "2016-09-24 00:00:00", "hostname": "www.andrewmaknco.com.hk"}, {"last_resolved": "2018-05-17 15:47:57", "hostname": "www.angelbluebeauty.com.hk"}, {"last_resolved": "2018-01-24 00:00:00", "hostname": "www.angelini-hospitality.com"}, {"last_resolved": "2017-11-02 00:00:00", "hostname": "www.angelinihospitality.com"}, {"last_resolved": "2017-04-05 00:00:00", "hostname": "www.anthonyblcheung.org"}, {"last_resolved": "2018-05-08 12:11:54", "hostname": "www.apexdesign.com.hk"}, {"last_resolved": "2016-09-24 00:00:00", "hostname": "www.arm.com.hk"}, {"last_resolved": "2016-09-24 00:00:00", "hostname": "www.artphoenix.com.hk"}, {"last_resolved": "2017-02-26 00:00:00", "hostname": "www.asia-packing.com"}, {"last_resolved": "2016-09-26 00:00:00", "hostname": "www.baby-lovers.com"}, {"last_resolved": "2016-10-30 00:00:00", "hostname": "www.beltone-hearing.com.hk"}, {"last_resolved": "2017-03-06 00:00:00", "hostname": "www.big-collection.com"}, {"last_resolved": "2016-11-18 00:00:00", "hostname": "www.bioprobeshk.com"}, {"last_resolved": "2018-05-09 11:38:38", "hostname": "www.bnsconcord.com"}, {"last_resolved": "2018-04-24 10:42:45", "hostname": "www.boa.hk"}, {"last_resolved": "2018-07-24 20:07:12", "hostname": "www.bop.com.hk"}, {"last_resolved": "2018-06-23 15:10:27", "hostname": "www.bt-links.com.hk"}, {"last_resolved": "2018-05-14 14:34:04", "hostname": "www.buzanhk.com"}, {"last_resolved": "2018-04-25 21:33:08", "hostname": "www.catbus-adventures.com.hk"}, {"last_resolved": "2016-11-28 00:00:00", "hostname": "www.cccklc.edu.hk"}, {"last_resolved": "2018-04-24 08:21:19", "hostname": "www.centralurology.com.hk"}, {"last_resolved": "2018-04-18 08:09:57", "hostname": "www.chant.com.hk"}, {"last_resolved": "2018-07-20 21:38:13", "hostname": "www.chinaworldtravel.com.hk"}, {"last_resolved": "2018-07-20 19:54:54", "hostname": "www.citipage.com.hk"}, {"last_resolved": "2018-07-26 18:38:52", "hostname": "www.ckskartracing.com.hk"}, {"last_resolved": "2016-12-08 00:00:00", "hostname": "www.cnf.org.hk"}, {"last_resolved": "2018-07-26 15:12:01", "hostname": "www.cplaromasfareast.com.hk"}, {"last_resolved": "2018-07-20 14:25:28", "hostname": "www.cwm-nethersole-fund.org.hk"}, {"last_resolved": "2018-07-24 14:26:54", "hostname": "www.deerhillbay.com.hk"}, {"last_resolved": "2016-12-02 00:00:00", "hostname": "www.dermanova.vizzhost.com"}, {"last_resolved": "2017-01-01 00:00:00", "hostname": "www.digitalmedia.hk"}, {"last_resolved": "2017-03-22 00:00:00", "hostname": "www.digitalonline.hk"}, {"last_resolved": "2016-11-28 00:00:00", "hostname": "www.diluxlighting.com"}, {"last_resolved": "2018-05-10 10:20:19", "hostname": "www.dsuccess.net"}, {"last_resolved": "2017-01-04 00:00:00", "hostname": "www.e-accounts.net"}, {"last_resolved": "2016-12-28 00:00:00", "hostname": "www.e-goodss.com"}, {"last_resolved": "2018-04-06 00:00:00", "hostname": "www.eaas.com.hk"}, {"last_resolved": "2016-12-16 00:00:00", "hostname": "www.ec-soccer.com"}, {"last_resolved": "2018-07-20 06:18:59", "hostname": "www.elekon.com.hk"}, {"last_resolved": "2018-07-10 19:54:51", "hostname": "www.entgulf.com"}, {"last_resolved": "2016-12-22 00:00:00", "hostname": "www.expert.com.hk"}, {"last_resolved": "2018-05-01 08:46:44", "hostname": "www.fastlane.hk"}, {"last_resolved": "2018-07-22 20:54:00", "hostname": "www.ferry.com.hk"}, {"last_resolved": "2017-03-24 00:00:00", "hostname": "www.garesch.com"}, {"last_resolved": "2017-03-07 00:00:00", "hostname": "www.geegeejerjer.com"}, {"last_resolved": "2018-04-30 00:30:15", "hostname": "www.generaliasia.com.hk"}, {"last_resolved": "2018-07-18 03:03:21", "hostname": "www.globegloves.com.hk"}, {"last_resolved": "2018-05-16 21:45:51", "hostname": "www.goldenratio.hk"}, {"last_resolved": "2018-04-29 10:37:20", "hostname": "www.hagerasia.com.hk"}, {"last_resolved": "2016-12-01 00:00:00", "hostname": "www.hangfuk.com"}, {"last_resolved": "2018-05-02 09:30:40", "hostname": "www.hangleei.com.hk"}, {"last_resolved": "2018-07-24 18:18:27", "hostname": "www.harvest-trend.com.hk"}, {"last_resolved": "2018-05-26 20:21:08", "hostname": "www.healthyme.com.hk"}, {"last_resolved": "2018-05-19 07:11:57", "hostname": "www.healthyme.hk"}, {"last_resolved": "2018-07-24 09:49:23", "hostname": "www.hkbcf.org.hk"}, {"last_resolved": "2017-02-25 00:00:00", "hostname": "www.hkjoyful.com"}, {"last_resolved": "2018-04-23 13:19:04", "hostname": "www.ideng.com.hk"}, {"last_resolved": "2018-07-24 06:15:08", "hostname": "www.interconcept.com.hk"}, {"last_resolved": "2017-01-25 00:00:00", "hostname": "www.j-zip.com.hk"}, {"last_resolved": "2016-12-12 00:00:00", "hostname": "www.jackwah.com"}, {"last_resolved": "2018-06-21 12:29:14", "hostname": "www.jameswong.hk"}, {"last_resolved": "2018-07-24 09:30:03", "hostname": "www.jungao.com.hk"}, {"last_resolved": "2018-05-27 05:33:40", "hostname": "www.kimberly.com.hk"}, {"last_resolved": "2018-07-04 10:54:01", "hostname": "www.kwan-tat.com"}, {"last_resolved": "2016-11-04 00:00:00", "hostname": "www.kwpgroup.com"}, {"last_resolved": "2018-05-01 23:50:16", "hostname": "www.lawrencelam.idv.hk"}, {"last_resolved": "2018-04-24 13:22:28", "hostname": "www.legendtoys.com.hk"}, {"last_resolved": "2018-05-07 07:49:58", "hostname": "www.lichton.com.hk"}, {"last_resolved": "2018-04-19 01:37:12", "hostname": "www.linkongkee.com.hk"}, {"last_resolved": "2017-05-16 00:00:00", "hostname": "www.logicworkshop.com"}, {"last_resolved": "2018-01-28 00:00:00", "hostname": "www.loongka.com"}, {"last_resolved": "2016-11-24 00:00:00", "hostname": "www.mamannbebe.com"}, {"last_resolved": "2016-11-04 00:00:00", "hostname": "www.masterclean.hk"}, {"last_resolved": "2018-04-22 06:08:46", "hostname": "www.masterkids.com.hk"}, {"last_resolved": "2018-05-03 18:20:21", "hostname": "www.maxhomes.com.hk"}, {"last_resolved": "2018-07-17 08:44:11", "hostname": "www.medequip.com.hk"}, {"last_resolved": "2018-07-25 08:54:40", "hostname": "www.mindmapping.hk"}, {"last_resolved": "2016-10-10 00:00:00", "hostname": "www.mso.hk"}, {"last_resolved": "2016-09-25 00:00:00", "hostname": "www.nelsonandcompany.com.hk"}, {"last_resolved": "2018-05-07 02:55:32", "hostname": "www.nelsonchtam.com.hk"}, {"last_resolved": "2018-04-26 19:07:09", "hostname": "www.neptunegroup.com.hk"}, {"last_resolved": "2016-11-08 00:00:00", "hostname": "www.nethersole-ss-ucnh.org.hk"}, {"last_resolved": "2018-07-22 07:39:54", "hostname": "www.newsound.com.hk"}, {"last_resolved": "2018-04-27 14:11:52", "hostname": "www.nextstep.com.hk"}, {"last_resolved": "2016-11-18 00:00:00", "hostname": "www.novanic.co.uk"}, {"last_resolved": "2018-05-07 20:05:39", "hostname": "www.nwpf.com.hk"}, {"last_resolved": "2017-01-24 00:00:00", "hostname": "www.oceangrace.com.hk"}, {"last_resolved": "2018-04-17 09:34:59", "hostname": "www.omnimax.com.hk"}, {"last_resolved": "2018-04-17 06:05:31", "hostname": "www.pilotstar.com.hk"}, {"last_resolved": "2016-12-11 00:00:00", "hostname": "www.pmpadvertising.com"}, {"last_resolved": "2018-04-24 09:31:44", "hostname": "www.poly-tech.com.hk"}, {"last_resolved": "2018-04-26 02:16:28", "hostname": "www.premierland.com.hk"}, {"last_resolved": "2016-11-19 00:00:00", "hostname": "www.redgoodss.com"}, {"last_resolved": "2018-04-22 18:46:18", "hostname": "www.regionfine.com.hk"}, {"last_resolved": "2018-06-29 12:43:34", "hostname": "www.richgoldman.com.hk"}, {"last_resolved": "2018-03-21 00:00:00", "hostname": "www.rwnt.com"}, {"last_resolved": "2018-04-22 13:10:37", "hostname": "www.sakong.com.hk"}, {"last_resolved": "2018-02-12 00:00:00", "hostname": "www.san-a-hk.com"}, {"last_resolved": "2018-07-16 11:05:19", "hostname": "www.scaa.org.hk"}, {"last_resolved": "2016-10-11 00:00:00", "hostname": "www.schaden.com.hk"}, {"last_resolved": "2018-07-24 10:21:53", "hostname": "www.servoair.com.hk"}, {"last_resolved": "2016-12-01 00:00:00", "hostname": "www.sh.americanclubs.org"}, {"last_resolved": "2017-02-08 00:00:00", "hostname": "www.sha-hk.com"}, {"last_resolved": "2018-05-22 11:40:39", "hostname": "www.sharewithyou.com"}, {"last_resolved": "2018-04-27 16:33:43", "hostname": "www.sharonhui.idv.hk"}, {"last_resolved": "2016-10-03 00:00:00", "hostname": "www.solarchina.com.hk"}, {"last_resolved": "2018-05-23 01:45:01", "hostname": "www.sunhingchurch.org"}, {"last_resolved": "2016-12-05 00:00:00", "hostname": "www.sunming.com.hk"}, {"last_resolved": "2018-07-19 02:07:51", "hostname": "www.toki.com.hk"}, {"last_resolved": "2016-12-16 00:00:00", "hostname": "www.top-pacific.com"}, {"last_resolved": "2016-12-18 00:00:00", "hostname": "www.tpshc.org"}, {"last_resolved": "2017-02-04 00:00:00", "hostname": "www.twowings.com.hk"}, {"last_resolved": "2018-07-08 13:19:19", "hostname": "www.ultraformgroup.com.hk"}, {"last_resolved": "2018-07-23 23:09:48", "hostname": "www.viewing.com.hk"}, {"last_resolved": "2018-06-06 22:08:37", "hostname": "www.viibiz.com"}, {"last_resolved": "2017-02-10 00:00:00", "hostname": "www.vingtsun-hk.com"}, {"last_resolved": "2018-05-15 04:58:29", "hostname": "www.vizz.hk"}, {"last_resolved": "2018-05-15 04:54:28", "hostname": "www.vizzgroup.com.hk"}, {"last_resolved": "2018-05-14 11:41:14", "hostname": "www.vizzhosting.com"}, {"last_resolved": "2017-07-10 00:00:00", "hostname": "www.waddyjew.com"}, {"last_resolved": "2018-07-18 22:52:56", "hostname": "www.wai-ming.com.hk"}, {"last_resolved": "2016-10-04 00:00:00", "hostname": "www.waiminghong.com.hk"}, {"last_resolv</t>
-  </si>
-  <si>
-    <t>{"asn": "40034", "undetected_urls": [["http://cripmotions.com/", "7b717a4848e28833c3d23c7d0768f4ae6eb02070c64aae8ae770da8982ad8a0b", 0, 68, "2018-07-26 07:00:05"], ["http://mikesnoodlehouse.com/", "dd461f01aabe85e537084302955dac4d40f735048eb1ae6edff4478eb0c2735f", 0, 68, "2018-07-26 03:40:18"], ["http://mp3linova.com/", "5df50733bc86b654089850cca011380120937e96f849881f25436e44b197237d", 0, 68, "2018-07-26 02:15:37"], ["http://dfeedly.com/", "6186ed2b632e9697d927f7d567e5a45e96b53f8682a8235556f9052e9014ac03", 0, 68, "2018-07-25 22:02:55"], ["http://moores.comvet-designs.com/", "4776b563eeab68f049bf7892f9462e5830b0517cf37dba366edc0f6c006855f6", 0, 68, "2018-07-25 14:27:41"], ["http://merketing.info/", "10d696ad1f23c9c875c73cf5cd6a451823931574c83d62dd812a8df037fd1e64", 0, 68, "2018-07-25 07:16:23"], ["http://huskersauthentic.com/", "2b498b1f407c81443ee35628b54bf36097970e8432e0d3e6bb4dbfa711c17c58", 0, 68, "2018-07-24 23:09:00"], ["http://www.theflapapp.com/GCM/OtherConfig.php", "e0fd51dc721a9eeb55c001692d4947dc18ea9634b7a814d9a329ea24533caf5a", 0, 68, "2018-07-24 10:55:23"], ["http://nullcoreproject.com/", "8c05f460f4538c0ccd63cd88a463ba2990c9cb3864ac4a3152af2dda13fe01b5", 0, 68, "2018-07-24 10:40:04"], ["http://searchpened.net/", "3a02210d6f684233044cf54610654dbb39f2faeebfc4e98f5fb6265cf388c690", 0, 68, "2018-07-24 01:44:13"], ["http://7knzz.survey3.curcer.com/", "0f005bed5824d5e58389db95dbfe0d3c78c4e7427c07d8310af4d59f5e96a432", 0, 68, "2018-07-23 17:48:39"], ["http://metralhas.com/index.php?blog=1", "74aa6cb0cec579b04adcd506c3cfafc66587d857fc4bcb1be47cffc9eb655872", 0, 68, "2018-07-23 17:26:56"], ["http://howtoremoveplantarwarts.org/", "d3047b94a21eb7e63abf281529c50da738d9b27a42c3195e8291aba11136fae3", 0, 68, "2018-07-23 14:51:40"], ["http://adupmediaxml.com/", "34c60ca8937f27f55f8498e01237e1fc6a8453c78192bc2a575f2a8fd7b80bf0", 0, 68, "2018-07-23 13:43:29"], ["http://me.quotelove.info/68/", "b719369217f8f00f119486b75c8e1f16471763b923b7a7e22d5fe91da473a4ca", 0, 68, "2018-07-23 11:45:23"], ["http://www.mobilsitelerim.com/Integer3", "4ba659e66c1c4a561372021d742730606773e6023628ae1f4083860989c92511", 0, 68, "2018-07-23 09:27:21"], ["http://fancycanes.com/", "08a631c313740912524e145e28b232d9489fb92431f48808bca72dba08b1a50f", 0, 68, "2018-07-23 09:07:01"], ["http://inkmeto.com/1-1emrpjtg7", "cd03fcbacd84d3b239d35708e31927721885d9ad050f0cd68e6255f7f23d0c55", 0, 68, "2018-07-23 02:04:21"], ["http://software4free2015.com/", "0e90b6b5af03131bbfddc47ce166ab711592beea51f6044df1bc2e7d27b681db", 0, 68, "2018-07-22 21:23:56"], ["http://thesecretsontheinside.com/", "5ac6a7bad74d7eaf06520f12e140d67a50dbaa3579485c74ac6157c843619e46", 0, 68, "2018-07-22 19:54:37"], ["http://tips4healthylifestyle.com/", "325008b90146169f50927f44f7003ee6278e936c2abbcc95d7e297ac1ae5be32", 0, 68, "2018-07-22 13:19:57"], ["http://ehowa.net/", "b802eafa0841122da30263c383f704fa15ab2f39b751b6fa9d1ebbdef85ef77a", 0, 68, "2018-07-22 09:31:26"], ["http://www.updatefastnow.com/", "3636ce00d86b5bfdac14c8767af3dc8b6214f93ab1b2c058b286bbb2da364af7", 0, 68, "2018-07-22 09:19:01"], ["http://www.laxmibahadurmaharjan69.000hostapp.com/", "d3f22d47d4b92b5b32b4a09fc08cbc652a0f599f7808b9f90b38c80521bf93da", 0, 68, "2018-07-22 07:47:47"], ["http://landscapingtipsonline.com/", "51e0e162a4ad4a3c5176c0a00f597647a8672b3ff4b0c3c8c965328dbe17a3ef", 0, 68, "2018-07-22 07:39:32"], ["http://girlsfanatic.com/", "cb94e30945a250e4eea65bb02161d28d3d9f04040123826458ba317682650ac5", 0, 68, "2018-07-22 01:32:45"], ["http://secure.imfbeye.com/", "9888ed86ad03b5023d65b7e5f6ce1a2b4990212ede0b1c177a8af0c2d854896e", 0, 68, "2018-07-21 18:25:29"], ["http://gaborcsupo.com/", "4fbae54682a71f19b49032e821db5322c95f8f13e754d042ce8173b95b2e7f5c", 0, 68, "2018-07-21 02:36:43"], ["http://www.eim327.com/", "d51168eba310d083124f739b880aab2f746fa4f787ad22af3ef435a854be6b3e", 0, 68, "2018-07-20 21:33:59"], ["http://jnj.condescosoftware.com/", "36a320f888be8d9343d12945d461926bf5395e87de6be967627e1fbd8f8c983e", 0, 68, "2018-07-20 19:55:40"], ["http://inkpcc.com/?repid=1074&amp;offerid=125&amp;sub1=k", "048fc9c6d27d5256de42162dc19f94292688b910ab699ac8261f3f83cc17ea01", 0, 68, "2018-07-20 18:25:11"], ["http://www.yasrarizvi.com/", "f5a82201344446cd31231ad2f274b262b220c79c0f9abe3e58ed0f7fbc8e4d95", 0, 68, "2018-07-20 16:42:04"], ["http://ebook.atusashop.com/book/cat_care_blueprint/index.html", "786af3f9c686dd2b81e2de86477e543991da048392ef9b76641c2588b79bb64c", 0, 68, "2018-07-20 08:14:36"], ["http://ebook.atusashop.com/book/positivethinkingasthekeytosuccess/index.html", "0047ca6b33972b1cbac2ac1664bba98348b95faf21799006eb2758613772e1e9", 0, 68, "2018-07-20 05:28:41"], ["http://pkn911.com/", "8dbe5242fa1db780d703f9d4b83b12632ec09f661f7d56c9be6c547cbcea333f", 0, 68, "2018-07-20 01:21:31"], ["http://indianpeacemedal.com/", "37da040c6e76f7f3a3d2a303401e564c684a403206c95f34b355cf156205f3ba", 0, 68, "2018-07-20 01:12:01"], ["https://071790.000webhostap.com/1.txt", "9a485d82f22849b3c0052bf2615ae4a74966b382b9eb5bd6fd86e879bdb5921d", 0, 68, "2018-07-20 00:15:33"], ["http://fx-chart.us/", "d6ddb882235cd6fa39c5b5c3496a27774226cfb6d0a84cbc4d2125c3fca51911", 0, 68, "2018-07-19 20:01:48"], ["http://www.hakdad.com/", "aab97d6cf8cf17b4cd2751b830a4ccd35d7115b56147844389c0d9e6be2b944c", 0, 68, "2018-07-19 17:18:27"], ["http://antiinflammatorysupplementsblog.com/", "f89509baf7b3d1b13beb1332c3e99f6ca77b22517d01770396062faf20f9c3a3", 0, 68, "2018-07-19 00:26:51"], ["http://work-center.org/", "a540ec21225af51cf40813b1933d2b16445d252313f317d8607256deea7daa0e", 0, 68, "2018-07-18 23:18:24"], ["http://cintasaccountsreceivables.com/", "b15262834f2d49fd32ba0fb8aad5c87bc2c54eb4b5db517a2bd28b9c559357f9", 0, 68, "2018-07-18 13:12:37"], ["http://manilaorientalmarket.net/", "bdb8928e091571783d413da299f16d4d29f0dc7a566825bf5e97b1d5b6737288", 0, 68, "2018-07-18 13:02:26"], ["http://consumer-journal-report.com/", "9e030a1142276c809903886225cb582bb2decd10b9a5ee965d9ce61f39ad1d3f", 0, 68, "2018-07-18 02:35:19"], ["https://www.freevbucks.com/", "543c21ed31213bf97f471fe8aea49eaf73e78e98f98b57f90e38fc678d4c03db", 0, 68, "2018-07-17 20:55:59"], ["http://email.nonreplymsdomain.com/", "e4fcbc44e37dc47465d89427e42e352a5030ba1cda987e39a81b462870c692d0", 0, 68, "2018-07-17 08:11:59"], ["http://unreached-worms.000webhosttapp.com/", "191ad4e3dda4fa89a0165f03f79d617cc1b6691d5358948f86d7f0f31da34c23", 0, 68, "2018-07-17 07:47:35"], ["http://www.viayor.com/", "dbb4cce1ce1bf310b2f383fd40ce97e1401c2551b39b8875e693f359c502866b", 0, 68, "2018-07-16 21:22:53"], ["http://www.freetattoopicture.com/", "c72de18d604707cafd1dd2a73595a6b97cbc162db6783f57174306acc6b8c32f", 0, 68, "2018-07-16 18:12:21"], ["http://nonreplymsdomain.com/", "9acae0e79f36c506fdddb8fb678f4d05d9707281b3c86bcf2e96309dacb1c3b8", 0, 68, "2018-07-16 18:00:28"], ["http://www.mrraymusic.com/", "78652840f44e4f33fab4f9a9796cea0afa426c44fee9cb74071264fb84564a48", 0, 68, "2018-07-16 17:28:02"], ["http://channel9newstoday.com/", "63d94e6bdd79411da63b5c8ef32162e0dec96441f0f0e6f8dbee1f0449dcaff8", 0, 68, "2018-07-16 13:25:48"], ["http://btintelligentsolutions.com/", "b11e13bfe77cb596fbd959c945892b6a0860c1b12eac884a882ea4aa379327ae", 0, 68, "2018-07-16 11:10:49"], ["http://dweluxe.com/", "005e9d9d81666460d7e7c19d7cf00d644e03a3fc91853ef01ff677ac72798298", 0, 68, "2018-07-16 08:26:20"], ["http://www.squdron.com/", "1388e1d482fa496c74541e22b90f66369e750479c88adfc86702e9c69c405696", 0, 68, "2018-07-16 08:25:16"], ["http://www.devletarsivleri.org/", "0aef41629bd840fab5e9fb1d224bfd9bf39a6504a5b1415a05b2fef61f3a57d8", 0, 68, "2018-07-16 05:51:32"], ["http://ebook.atusashop.com/?ga=6KNX5%2FuvmNOPzSY6NrtEBMm3CCmgYt8LC%2Fxaf2kqLLk5MQyqcRJn4MbFvnD0zZ4PmlUPRbGBxzxOWl4c%2FZp9judKW0Y5gB9PxnmPjqzjgq3ejjqVk430%2BaX56TMMMcjm66S3oZ0NT0Rybla7qLMcdw%3D%3D&amp;gerf=VagFo0AjxMGlj1JWGEzed%2BkRTFj5rBvf6Lt695kUn2k%3D&amp;guro=s40Ts9EeJ3FfTyjTIfx1sd9kZ6EO7V%2BFehlIxFraJwpF%2F%2B3C36jYtNn2kTRkcUUTYNUOZilyoLM2QCcnULxlQQQg5mIUqnOfuMzKttADCn8%3D&amp;", "d7d9420339969b33b6922b4f2ac2285c99c3bd896e82fcba8789684e1cc9ddd5", 0, 68, "2018-07-16 02:33:05"], ["http://message2bx1.com/", "fa65c03ced5bac8cddfe9c91f3258e4167313130d7c1e686a04986ebd52fe9a4", 0, 68, "2018-07-16 01:30:34"], ["http://starmoviestream.com/", "0b35ddc40a495a9f34b304598ca3541983498bee6d5d60ed2424767311a97137", 0, 68, "2018-07-15 18:30:25"], ["http://bufferstreamz.com/", "fda3a694ad780ba59b13d931501a03430f5996024d496c88fca10d60b399b884", 0, 68, "2018-07-15 17:39:47"], ["http://privatecaminvite.com/", "1bf4c3c8fd1c3b1c9405465c317cb2b722b3d49f7c7ccc2e41e9aabca4a935da", 0, 68, "2018-07-15 13:20:06"], ["http://amulyabharat.com/", "51b07dce23d6aec4a37c5a1ec6c795a7b0e4fb938a6b975873764471401b7a43", 0, 68, "2018-07-15 12:30:42"], ["http://oceanpdf.com/", "e727ae45a46f9835a346ff9df1487067f96743a5326b44c302c7762efac47e2d", 0, 68, "2018-07-15 12:12:50"], ["http://emeralbux.com/", "10c612caaf57b3495edcc24cef1309170db3ac4084635634858cdbd7661154de", 0, 68, "2018-07-15 11:48:02"], ["http://apprenticeprideceiling.com/", "a51c95bc29c629e19d23985eb48c1a12a46c5df50aa7bbd4d61fcf6ae32e0324", 0, 68, "2018-07-15 11:29:14"], ["http://zipansiom.com/1zUBs", "805dce4b1cc79031922d7233d5726119c3e283a2af3cd6760db1d4d277e7e26d", 0, 68, "2018-07-15 10:44:26"], ["http://codefinder.net/", "2bdd4c73acae7f2cfeefd636b6f19116d434968fa8eaa4ba8e3c6bda24861076", 0, 68, "2018-07-14 22:45:16"], ["http://filmon-live.com/", "c984f765e0ede187b1202ad15ae75e551397a8347ff9f16c0e7174ad6e6103d9", 0, 68, "2018-07-14 19:33:48"], ["http://businessplanlibrary.com/__media__.....F?url=https:/belezanaweb.info", "39edc865f9073d44e598f0ece4cf5ff61fb1a293497beca292cd43208eb00efd", 0, 68, "2018-07-14 13:02:05"], ["http://inkpcc.com/", "f47b3cb56ddc10958a13e5a04d77f5045227721153f7356749b93bc951421e21", 0, 68, "2018-07-14 06:40:57"], ["http://bollywoodceleblist.com/", "cfcdd1fccae1355c1f6ddd049edc424565e2eafb1de0577f4b2e51ad4b92052d", 0, 68, "2018-07-14 01:18:18"], ["http://fortniteporn.com/", "d9c1926f547ed20984646a6fef540cbb21714afe0300aee5c571f91d462003d8", 0, 68, "2018-07-13 23:32:08"], ["http://crackingpatchig.com/", "fcc647589de88ddcd08e310a8cf6d91dd9cbc83c5aad136142dc2a7e15f1e222", 0, 68, "2018-07-13 17:09:36"], ["http://exercicespourlesfemmes.pimpstore.info/?ga=idQ1gtJhpJBM93CmhFekDQ%2BZuJjD8n6yBEzGGmWK23RuJ5jQDMMGdXSumdP3vrFr%2FZT%2F%2B%2Fsr2Ra57Pt9W2n42fC0MY10pC%2Bm0Ko%2FpLemWaftGBfIOkTXXZFh6oXeXU6foXQS%2BB%2BNbtwNrf6WtaSpiA%3D%3D&amp;gerf=NqDRDRdaDUCegHij3ek0odBBnWHPbKup1NmvIpyZQmQ%3D&amp;guro=we4mb4V0glAHoqrP%2FrgtKclfuHHrEjGxUecclk4SxR4uh0RO%2B7MUU5N9kG0zOvnQezMD0S%2BUdMe%2BZKoLY23lEg%3D%3D&amp;", "fdb22d1bf33763767bd48afb44aa4f3c01c4b0a7a68ddf0750c1d58bef7a30a2", 0, 68, "2018-07-13 13:36:10"], ["http://pricelesschange.com/", "da556d196cbd969aa9eef38789687ffb8e018fe59c72746fd78a8eede2862457", 0, 68, "2018-07-13 12:56:44"], ["http://ns10.aqgsi.info/ipadcn/ipad6.html", "d770975d3bb0a726f32b4f504556f0e23204ca63d19b98f57cf7a2ffb2e26c3d", 0, 68, "2018-07-13 05:57:52"], ["http://gsgfsdgfdhjhjhj.com/", "ee059ca6833ee4107af5481721bb2d3b01aaca2f7625728ab435235c3f474c6c", 0, 68, "2018-07-12 22:33:18"], ["http://jpsdesignbuild.com/", "467f691d45ec0a56394f410de6947129a92e86043c1ed19989b236e6af5038bd", 0, 68, "2018-07-12 19:49:33"], ["http://www.javfin.com/", "8e7cb2229adcdb598ba366ec8b601018aed50f3e2b12bd2bf340d87dc0db4e53", 0, 68, "2018-07-12 14:15:46"], ["http://ebook.atusashop.com/?ga=5RrATQzHH9VFyXhVhKKPQNgIdZ6RnhCnMDsGBKyEXmwAyRYKgwJtZIIQbpEzZlSwjehcbn0Z2zFRNLnZo09zQGkQ5fraCeLtDisikkFFF9i5a2uTKl8jzUcUQfs4db1zmkN3sUQMo5U8N3JE%2BADmXg%3D%3D&amp;gerf=I2G4E8ofI%2Fvza3GHBQ8YoRqiIGaNgDsw9JIqmla6hiI%3D&amp;guro=yd4iypW8l%2BbrjUNvDL%2FPD8CNKsM%2F3o7MPf8FMIpGNLE93QBsJfoELyPUCFD6EamP4RxQ6M3esHlvoO3rFx7qAaLIN0zOuA7AQu%2FjOB5KViI%3D&amp;", "ab8e0340b7fbb736898e8a854aec6548a61faa418c9f79cc97e3e655075a698e", 0, 68, "2018-07-12 10:22:59"], ["http://www.onlinevideosdownload.com/adpintretarget.php", "3d4ab8b7a3e791a1d2817cdff1aa245ffc53e983bce40697526357a54f820ce6", 0, 68, "2018-07-12 03:42:24"], ["http://ebook.atusashop.com/?ga=HTLOAtYLXMbvzYyGmNpSbg62jm9IdVn6B8j%2FRtCbmNZUEbnDxW48yhpb39NAk0t6jp62WegRvPpfwksijBWNH0U6eEmb4gz0cuNWuUtL8DNbHoiTiOhN5spnad7Q7SxkKihmU5AcGnkgofl0FBGGfQ%3D%3D&amp;gerf=odS5AsVY1lVIB53pc2xuG%2FIQ7%2FV1YER1Llb3boAcoPE%3D&amp;guro=6smgUgw1FK5AVl5TQ%2F7mn5AIWmp%2BBIKgAx5NiNtsA4shCN8t%2F9GtioZq1xsYRruj8yVBsxc5AErBHvVeS0jzO%2BnxZ%2FeQJwqVcTJsRLLXP4g%3D&amp;", "d9a3b7b93eb9d6efecfcfe9f44b25eabc5f91aa1c14cc2f8b5170f68d28a2de2", 0, 68, "2018-07-12 02:24:08"], ["http://www.partvull.com/", "fa8b4bd9e36e120a295a6c2820ded2ea0ec33dc76964c6dd93271a4e384ba252", 0, 68, "2018-07-11 23:48:52"], ["http://quiizziz.com/", "f6b2396ec362791c346879cf4865a66d8aaa43769562184a89af15da5e6fd8a8", 0, 68, "2018-07-11 21:35:12"], ["http://judgmentinvesting.com/", "088ef639c7c9e47c4d4927c36bb0e6c1692a88fd0105bc951418eea495440517", 0, 68, "2018-07-11 21:23:47"], ["http://www.krava.org/", "985cf1e3f8ab1d0d287d8629e8aa7f1e274fdf8ffec86964d4d0eb97021332cc", 0, 68, "2018-07-11 21:19:44"], ["http://manilasouthcemetery.com/", "4a2d0918138c1c2558ef2a34067b7f0f508853df46651af0f6454f1faf8cd322", 0, 68, "2018-07-11 20:01:15"], ["http://christiekane.net/", "2ee6abbff3bc9717f6b4008bf2b337387f11bbf9c81e51697b163a8e453369ba", 0, 68, "2018-07-11 19:11:12"], ["http://sseimaging.com/", "e17f274fd4bfd551dea123e2ba8bc29839585aa1c76efe0928d3aeacc223b4c5", 0, 68, "2018-07-11 19:09:13"], ["https://florida.pnpaware.net/", "d97d3e177c701750fa71fb3bd94b16cb9ccfa411e0bf481c6f63835a9e5dcca8", 0, 68, "2018-07-11 17:43:37"], ["http://shenandoahshepherdrescue.org/", "e1ae660c56a7ce6ed66221955818beb2664b416a22cfc532b99c3fc120f7c556", 0, 68, "2018-07-11 17:13:00"], ["http://elsprofessions.com/", "66580496681ba740e7326ac06052e034a860c243b360a6326aff156581cf8fba", 0, 68, "2018-07-11 16:11:28"], ["http://partmentfinder.com/", "8a057ff207f9b72d007d49619a4332596ae788a629225c7d4c565f506baa62aa", 0, 68, "2018-07-11 10:54:00"], ["http://missimple.apcprd01.prdexchangpe11.net/", "cd9d35cde266dd63d8d424bf0c0b7e2656ec6ab7c553970851bedbccb29c6799", 0, 68, "2018-07-11 10:09:34"], ["http://microformulas.com/", "d4d238d682fc34e5ad79e271f3f461e129fcbb84887ce94939c709cdcde24edc", 0, 68, "2018-07-11 09:12:01"], ["http://gaggit.net/", "60e186fa1eb3f7984ac088685922058a2d9512111e9c351244dce96b6793addf", 0, 68, "2018-07-11 04:52:03"], ["http://httpchelsinkifashionweeklive.com/", "41e5434c77165fb817040a3d57f7cb34de4bd1056f48d6cea8ad1daa44af4623", 0, 68, "2018-07-11 02:36:59"], ["http://ipaymentcompany.com/", "1600ec0d33df98fab8f00534dfd967dde0531f0eedbb348ae2b8413fa90b939e", 0, 68, "2018-07-10 20:25:29"], ["http://www.badumtss.net/favicon.ico", "55c79afeaaf41af8f9fa163bebfa11b1a8204ab653e63e941e4b95566b1e0434", 0, 68, "2018-07-10 17:30:48"], ["http://pop3.nbtank.com/", "98db383fc675b2507e41c715231c2e61db57c4c1f7993c9dabc760ba1d244d67", 0, 68, "2018-07-10 13:48:25"]], "undetected_downloaded_samples": [{"date": "2018-07-26 18:09:02", "positives": 0, "total": 59, "sha256": "083d15a07f8702e1216f5ec39ee1879d1459e307a6ee7ae223651fed856dae93"}, {"date": "2018-07-26 06:17:05", "positives": 0, "total": 59, "sha256": "c75eb01138771bfb2a5517aeae882356733782767c4560cc9601c34d2591ca75"}, {"date": "2018-06-13 04:21:54", "positives": 0, "total": 70, "sha256": "e050ed0c2c119e39f9bbf2819a92c076b2efeaeadce7c3d4deaa5fd5657b9e3b"}, {"date": "2018-06-04 07:22:28", "positives": 0, "total": 56, "sha256": "1c6f11f4cddee66a9b20a0aaa66e2d024a3a12092f0a501510fd8ccdb6867065"}, {"date": "2018-06-01 12:28:50", "positives": 0, "total": 71, "sha256": "e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855"}, {"date": "2018-06-01 10:56:37", "positives": 0, "total": 50, "sha256": "8f0a3bbb3b421ec55165a5807352018938101494dc37c49c3e5c407ce048256e"}, {"date": "2018-05-31 05:10:23", "positives": 0, "total": 55, "sha256": "fa2bf64baf8b8187dc1d0a0cbce0b8d4d18debc8f15a6a7b42b38f0a87d0db12"}, {"date": "2018-05-30 10:35:31", "positives": 0, "total": 57, "sha256": "2069234b01e33ec7e8f4a78edad8a3909501233d6860f87855981f49992e06a1"}, {"date": "2018-05-30 05:50:03", "positives": 0, "total": 54, "sha256": "253952a3d9de484f2d40a3a5e013c3fa29b436e21dc91dbb520eaa092c120509"}, {"date": "2018-05-14 22:20:10", "positives": 0, "total": 60, "sha256": "5c1d5fd46a88611c31ecbb8ffc1142a7e74ec7fb7d72bd3891131c880ef3f584"}, {"date": "2018-05-14 07:38:05", "positives": 0, "total": 59, "sha256": "1e02bafd3076f95b9469e058b1eeeab3501e3c97fc6e1f4e577c82622af2ba90"}, {"date": "2018-05-13 19:03:21", "positives": 0, "total": 60, "sha256": "3a08352e67466b2575cc8a910523ab801c3e6c45d9fe172119daf290e190f6c5"}, {"date": "2018-04-04 09:17:15", "positives": 0, "total": 58, "sha256": "16c2adc9da7d96029f878cebd9fd51caddf48e131925a415461aa05b2f7bd675"}, {"date": "2018-03-30 04:27:53", "positives": 0, "total": 60, "sha256": "1d07d3578b789e6c94af47e8ea6d7b1982e8341f67c9a4de2709189d5b93515f"}, {"date": "2018-03-28 16:20:33", "positives": 0, "total": 57, "sha256": "f935be28fc7923062315766f13f82a54281409c35abc76a16f731539e08f62d7"}, {"date": "2018-03-14 07:12:52", "positives": 0, "total": 60, "sha256": "d3a36f55a32cef1a822dbeda312e521826195788fe9bf48011d93b73e94c6956"}, {"date": "2018-03-12 04:10:09", "positives": 0, "total": 60, "sha256": "e169c565be92b31e8d93161b0758c01abddb4c5f1ec0aa20bff5258d882c0d1c"}, {"date": "2018-03-10 03:55:51", "positives": 0, "total": 58, "sha256": "18dc4f505d6d9132f8e76d6ef7b0c9281c9324f3349cddf957db13dcddc46c97"}, {"date": "2018-03-09 03:27:38", "positives": 0, "total": 60, "sha256": "0dafae0232667b7736934090604a23d9328d29d2d3c62fa9048a89368b140679"}, {"date": "2018-02-23 02:29:31", "positives": 0, "total": 59, "sha256": "e1b7a04ea31b204cdc3f299994f6042a789381da90d98245e7cf20d6afad79e9"}, {"date": "2018-02-22 22:05:03", "positives": 0, "total": 60, "sha256": "c1b03007296d41daa264a4c41cdeb795959b51443110529486141442f074a8d8"}, {"date": "2018-02-13 05:04:35", "positives": 0, "total": 71, "sha256": "e80c90fbefe1cbd1b629c71ae1f313f8df0ea595d5295a5f8fc99b291f9874df"}, {"date": "2018-01-29 03:29:35", "positives": 0, "total": 67, "sha256": "33064c2f8ece443cbaef034a427b86f435f279b1a18a1bb0ef4074c2055612e9"}, {"date": "2018-02-10 23:25:11", "positives": 0, "total": 57, "sha256": "5b0f86a4c9c9ff2ec90a319d2076f00e706ea68a8436565cdbae46c04de0a4db"}, {"date": "2018-01-30 01:59:54", "positives": 0, "total": 69, "sha256": "e8b1e6a2a0b3caa7de87c863fdbf1293474cdd28f4d8dd5f4ca80da019a2cf9f"}, {"date": "2018-02-04 12:01:05", "positives": 0, "total": 55, "sha256": "0f7887ae923b6205836fbd3e394ae8782e1775411bdac5a034d8d9c890f7a761"}, {"date": "2018-01-27 00:41:52", "positives": 0, "total": 56, "sha256": "e64e2f4d8a4e8767c99ed87708c6af4fd424031bc933e2a0553aa7235903bc51"}, {"date": "2017-12-03 06:17:53", "positives": 0, "total": 49, "sha256": "71eec56eed73830f28f570eb33a348e447bca71770ae1ad9b959cd59bfa3d906"}, {"date": "2017-11-12 18:51:57", "positives": 0, "total": 60, "sha256": "50b9564126c24a40212bbf846817b515a3a4a5440b0c993e99c271b1b9c33cde"}, {"date": "2017-10-26 12:19:49", "positives": 0, "total": 56, "sha256": "e10aa5cfb3a2675cfb50f056b3c0b1b08e96f4ed5da21c4a7744773374e35fbe"}, {"date": "2017-08-15 05:32:04", "positives": 0, "total": 55, "sha256": "123069fed711743dfc5f24af4f8cb494ff130db7cd387f45e225d6c3ba9548c5"}, {"date": "2017-06-27 06:32:08", "positives": 0, "total": 57, "sha256": "0c2205b19d377415bbd5919f3ffa2ffd5b812320eb408fe70190bc1f83cfbe35"}, {"date": "2017-06-21 21:43:54", "positives": 0, "total": 56, "sha256": "7f6abeabefca5b71b2f10cd25a3a2d3712772ca22f392e974941172ece6f6e23"}, {"date": "2017-06-20 21:55:27", "positives": 0, "total": 56, "sha256": "35dd91c63a63f4bc2f1467777ce8898c9e36f9a4f1ddd84c65d049189e2fd170"}, {"date": "2017-06-14 13:17:46", "positives": 0, "total": 56, "sha256": "ffbe6305a1f927a1dea3714a8c469d31695657124eee341d5b21f6d255c8cb13"}, {"date": "2017-06-14 07:14:03", "positives": 0, "total": 56, "sha256": "fcc59fe507792134acabf0a956ae163ebbffba66d405bc4fb176300778299654"}, {"date": "2017-06-14 03:54:10", "positives": 0, "total": 56, "sha256": "c6397516effa6c5446baf0e48067f3a11f1339b781e35918e293eaa6d9b77c5a"}, {"date": "2017-06-13 07:56:34", "positives": 0, "total": 56, "sha256": "4e215649293d8adf37c22fd971f448c18476838efb8eddc222ff606f01b7f908"}, {"date": "2017-06-12 21:00:20", "positives": 0, "total": 57, "sha256": "45dd8bae67502c44238048dbfd607e654a36b893e03c4281e0d8be5872ba8758"}, {"date": "2017-06-04 13:30:52", "positives": 0, "total": 57, "sha256": "07dc2f63c24244a29bef303a40e43e36cbc589c205994b5d5a10adf8d17e4c49"}, {"date": "2017-03-31 11:43:54", "positives": 0, "total": 56, "sha256": "e7430da8fb09dd5905088762e4f17d1050438ded1846ca7e405346d8d1958f79"}, {"date": "2017-03-20 19:43:26", "positives": 0, "total": 56, "sha256": "a63e40285ce0e6d9a014372142c7360a3601609466173c12bed0e10c2cebb90d"}, {"date": "2017-03-20 17:02:07", "positives": 0, "total": 56, "sha256": "000a7960376ffd28bf179bd1d986b66288870dca21c23defb2bc762c475b0001"}, {"date": "2017-03-19 14:44:37", "positives": 0, "total": 56, "sha256": "f450e511148310cb286638b70e85ba752f8a7e140d563c2446b87aee05b4d330"}, {"date": "2017-03-19 11:26:37", "positives": 0, "total": 57, "sha256": "070e6396d00d24041a40012621d7925e25f3b5d8a04b85be5d5cb7d79c06e6a2"}, {"date": "2017-03-18 11:57:54", "positives": 0, "total": 56, "sha256": "53d1e17a1a7bf31cb01039e29d5806f739f2e3efaaca3a44f86081fe5750b929"}, {"date": "2017-03-17 22:27:55", "positives": 0, "total": 57, "sha256": "7b5dd3e9071356876737be54e82db644eaa6cef1036d563882f1ffca22829088"}, {"date": "2017-03-17 19:23:48", "positives": 0, "total": 56, "sha256": "0c78bf418c471b26f3c54c378649c78d6b2dde4ae0d2c68ff79e65ec8d6ff0dc"}, {"date": "2017-03-17 16:21:46", "positives": 0, "total": 56, "sha256": "ac8a9f990bcba855d74a550cb2e7036885cad5b745a2a38730d2e5e21f5633db"}, {"date": "2017-03-17 12:44:16", "positives": 0, "total": 56, "sha256": "8c1dfa3ef0c2e3861f5ea3b90dd0a8ec511424c74ce44cc7bb0f89a02bcc47e4"}, {"date": "2017-03-16 16:26:13", "positives": 0, "total": 55, "sha256": "6f2686a3582de308918f4ea019c4325ec50fdf5165206e836916d6211190d9d8"}, {"date": "2017-03-16 15:29:07", "positives": 0, "total": 56, "sha256": "cf4b7ad62f1c517d40ac1b160e4e227e94e9d842993a39239bf24ed3a44f40be"}, {"date": "2017-03-16 13:12:03", "positives": 0, "total": 54, "sha256": "7376690c99515140ca86e992d5e775ca672e637a04a0d30a7a4a78341ee786c8"}, {"date": "2017-03-13 13:26:21", "positives": 0, "total": 54, "sha256": "c4ae392319a178c3444fba5f77fb09bef4dca814a3526f5924db82bc2f8923ae"}, {"date": "2017-03-01 17:53:48", "positives": 0, "total": 57, "sha256": "2854538005dc5335f774570e22360fe1c96dfb6b5d5105cf93a675d7ccceb365"}, {"date": "2017-03-01 06:06:50", "positives": 0, "total": 54, "sha256": "3941d23372783c14a7f79b2a2a0d5ab8a88ad385979ada0e23255aaf67aac7a5"}, {"date": "2016-12-14 18:42:30", "positives": 0, "total": 56, "sha256": "543f795965b1c0f6c60425bbdadebfaf78eb14fbc414580ec72c47a441a0ddf1"}, {"date": "2016-10-03 15:58:24", "positives": 0, "total": 55, "sha256": "3eb10792d1f0c7e07e7248273540f1952d9a5a2996f4b5df70ab026cd9f05517"}, {"date": "2016-10-02 09:59:06", "positives": 0, "total": 56, "sha256": "9f9a85601ab426bef07a9f33590521b8d21a529fd799f2d4cb9e4daabd6abdc3"}, {"date": "2016-08-28 09:07:41", "positives": 0, "total": 57, "sha256": "61173b77fa33cfa203e4dc5565dc5c26a7022c65c3f4ef7ec8b566ebf9c0b98c"}, {"date": "2016-06-01 21:46:55", "positives": 0, "total": 57, "sha256": "7f749ede2054533ce24c872d62cd88b39e321202587c4f85c66ac40ba43daed5"}, {"date": "2016-04-25 04:05:11", "positives": 0, "total": 56, "sha256": "7c470d8f0878b9dd785934f51399ec29b1dd6538b46fa7f2f0bc462d21be98cd"}, {"date": "2016-03-13 05:15:38", "positives": 0, "total": 57, "sha256": "e75fb19a6e167b6bf5b614e9ca4df333f9b3bd06edb5ea0a7cb60d19cb789065"}, {"date": "2015-12-25 22:56:59", "positives": 0, "total": 57, "sha256": "2f34354accc2ca60a05680edd1c1e2fc065a8d245227d8ab52b1123c7ece5506"}, {"date": "2015-11-01 11:51:16", "positives": 0, "total": 54, "sha256": "108474fc7eaff1d180eead2038c3cccbfc5e77446e9877e56e7ddf9cb14a3869"}, {"date": "2015-10-26 03:23:49", "positives": 0, "total": 56, "sha256": "80fad2614fa13e28612bf615f0b91301401d674e3a7bd7652dc49de739135c3d"}, {"date": "2015-10-23 15:02:08", "positives": 0, "total": 57, "sha256": "36bdd8284447c4bcd4f1b1a4d5d2b1513ee2ba8815beddcab2d85d3dd2f8700d"}, {"date": "2015-09-25 00:25:03", "positives": 0, "total": 56, "sha256": "5b12273e558d1ac0ca8a8f5d6fa46aff073c389c9c7b6ca4c653914ba6e26317"}], "country": "CH", "response_code": 1, "as_owner": "Confluence Networks Inc", "verbose_msg": "IP address in dataset", "detected_downloaded_samples": [{"date": "2017-12-04 01:39:35", "positives": 1, "total": 59, "sha256": "f2b7555ae5e1c944d0b12955ae93e2de65515247867af6951da6747a357003ae"}, {"date": "2017-11-12 10:41:36", "positives": 2, "total": 60, "sha256": "37d208478f81cd49e083c212c61b8fd75e4006e2085b1efd7238d2ff482f9048"}, {"date": "2017-09-21 04:25:22", "positives": 1, "total": 57, "sha256": "586d7d0759b46647648889ee6a1a327205885cbf3dbacef914371d0b49c72461"}, {"date": "2017-08-03 11:15:07", "positives": 1, "total": 59, "sha256": "6c206740afc2516a88b38494beeaab07ff5ea9a697879254f4faa72433a12a98"}, {"date": "2017-02-04 15:29:14", "positives": 1, "total": 55, "sha256": "4ba1a0fcc6983b539744a6590920fc4596460833c306bb1531095ada391ab21f"}, {"date": "2016-04-18 02:23:36", "positives": 33, "total": 57, "sha256": "3fc8056f935d395cfde5867ec4f95396e612626e7d8ad4125392e9a227b1c0e9"}], "detected_urls": [{"url": "http://paypal.co.uk.userz8oh8cp6hvo.settingsppup.com/id1/?eml=&amp;cmd=form_submit&amp;dispatch=34xsd45423d1zmw241234zxadvzvh24af23d60", "positives": 8, "total": 68, "scan_date": "2018-07-26 20:52:12"}, {"url": "http://lastversion.safesystemupgrade.net/dl.php", "positives": 3, "total": 67, "scan_date": "2018-07-26 20:33:29"}, {"url": "http://www.manice.net/index.php/glossary/35-server", "positives": 3, "total": 67, "scan_date": "2018-07-26 20:03:28"}, {"url": "http://files.fastdld.com/v1.5/click/eado2ny6/?filename=setup", "positives": 4, "total": 67, "scan_date": "2018-07-26 19:50:30"}, {"url": "http://www.homestosellmn.com/?p=431", "positives": 1, "total": 67, "scan_date": "2018-07-26 19:49:28"}, {"url": "http://stufftodoinnyc.net/thin.php?largest=659uu6cwxhznrmcg", "positives": 2, "total": 67, "scan_date": "2018-07-26 19:48:37"}, {"url": "http://766-diet.com-gem.net/docszmo/enszmo", "positives": 4, "total": 67, "scan_date": "2018-07-26 19:42:23"}, {"url": "http://b.api6.net/inputInstall.php?subPrefix=fl6u6v2sdlc&amp;idDevice=2&amp;mcc=460", "positives": 7, "total": 68, "scan_date": "2018-07-26 19:31:11"}, {"url": "http://411-weightloss.com-gem.net/docdfvk/endfvk", "positives": 5, "total": 67, "scan_date": "2018-07-26 19:09:24"}, {"url": "http://510-beauty.com-gem.net/docamjb/enamjb", "positives": 5, "total": 67, "scan_date": "2018-07-26 19:09:22"}, {"url": "http://fu-mak.com/", "positives": 7, "total": 67, "scan_date": "2018-07-26 19:02:56"}, {"url": "http://adobe.com.biledeosd.com/", "positives": 4, "total": 68, "scan_date": "2018-07-26 18:57:58"}, {"url": "http://alert-mobi.com/", "positives": 3, "total": 67, "scan_date": "2018-07-26 19:02:53"}, {"url": "http://pedroportillo.com/", "positives": 1, "total": 67, "scan_date": "2018-07-26 18:33:53"}, {"url": "http://mars.beautyspaguide.com/index.html", "positives": 5, "total": 67, "scan_date": "2018-07-26 18:28:50"}, {"url": "http://mylearnigplan.com/", "positives": 1, "total": 67, "scan_date": "2018-07-26 18:19:35"}, {"url": "http://appsom1.com/ppi/click-wib?dp=5036", "positives": 4, "total": 67, "scan_date": "2018-07-26 18:15:20"}, {"url": "http://localleadexaminer.com/wp-includes/SimplePie/Decode/HTML/supportredirection.php", "positives": 4, "total": 67, "scan_date": "2018-07-26 18:09:46"}, {"url": "http://alcachofadietampolletas.com/wordpress/wp-content/themes/atahualpa/images/favicon/new-favicon.ico", "positives": 1, "total": 67, "scan_date": "2018-07-26 18:08:58"}, {"url": "http://gamecomes.org/template/TrinityPurpleOneClickCAF/search-bg.png", "positives": 4, "total": 67, "scan_date": "2018-07-26 18:06:37"}, {"url": "http://gamecomes.org/template/TrinityPurpleOneClickCAF/main-bg.png", "positives": 4, "total": 67, "scan_date": "2018-07-26 17:59:32"}, {"url": "http://compsecurityer45.com/", "positives": 2, "total": 67, "scan_date": "2018-07-26 17:42:11"}, {"url": "http://verify-manage-additionalcontrollers.com/", "positives": 2, "total": 67, "scan_date": "2018-07-26 17:30:29"}, {"url": "http://683-fitness.com-gem.net/docklim/enklim", "positives": 5, "total": 67, "scan_date": "2018-07-26 17:11:02"}, {"url": "http://b.api6.net/inputInstall.php?subPrefix=fl6u6v2sdlc&amp;idDevice=2&amp;mcc=405", "positives": 7, "total": 67, "scan_date": "2018-07-26 17:08:36"}, {"url": "http://257-healthandbeauty.com-gem.net/docmjwp/enmjwp", "positives": 3, "total": 67, "scan_date": "2018-07-26 17:00:50"}, {"url": "http://461-weightloss.com-gem.net/docqhia/enqhia", "positives": 4, "total": 67, "scan_date": "2018-07-26 16:56:42"}, {"url": "http://keyupgrade.safesystemupgrade.net/dl.php", "positives": 3, "total": 67, "scan_date": "2018-07-26 16:17:34"}, {"url": "http://gestiondeempresas.org/wp-content/plugins/jquery-image-lazy-loading/js/jquery.lazyload.min.js", "positives": 2, "total": 67, "scan_date": "2018-07-26 16:16:26"}, {"url": "http://apple-greens.com/b/eve/06a0a5de211e2318043f5d21/", "positives": 3, "total": 68, "scan_date": "2018-07-26 16:00:09"}, {"url": "http://crdghh.net/", "positives": 5, "total": 67, "scan_date": "2018-07-26 16:02:57"}, {"url": "http://oriru-han-er.com/f/fide/index2.php?log_in", "positives": 7, "total": 67, "scan_date": "2018-07-26 16:02:52"}, {"url": "http://missmaker12.com/support/tunes/car.php?cmd=_account-details&amp;session=bca0ea1e4e57616fb3401b94e0974f54&amp;dispatch=0d6f08f3891223aa08f629464c2053f1b48a8175", "positives": 8, "total": 67, "scan_date": "2018-07-26 16:02:50"}, {"url": "http://acunuryphrgritedsjusinuslimtablens.com/", "positives": 5, "total": 67, "scan_date": "2018-07-26 16:02:48"}, {"url": "http://ready4live.safesystemupgrade.net/", "positives": 2, "total": 67, "scan_date": "2018-07-26 15:25:08"}, {"url": "http://breezalite.com/cutting/thefuck.html", "positives": 3, "total": 67, "scan_date": "2018-07-26 15:24:22"}, {"url": "http://top-free-app.com/", "positives": 7, "total": 67, "scan_date": "2018-07-26 15:03:17"}, {"url": "http://www.globalinsurancenow.com/wp-admin/maint/admincp/a3b6233dcdbe5e04671ccb57d6f62353/key.html", "positives": 8, "total": 67, "scan_date": "2018-07-26 15:03:16"}, {"url": "http://leoperfu.com/", "positives": 6, "total": 67, "scan_date": "2018-07-26 15:03:12"}, {"url": "http://files.fastdld.com/v1.5/click/3ef7583f/?filename=setup[]", "positives": 3, "total": 67, "scan_date": "2018-07-26 14:54:27"}, {"url": "http://729-beauty.com-gem.net/docyjuc/enyjuc", "positives": 4, "total": 67, "scan_date": "2018-07-26 14:30:55"}, {"url": "http://www.homestosellmn.com/?tag=minneatpolis-suburb-condo-loft-for-sale", "positives": 1, "total": 67, "scan_date": "2018-07-26 14:21:26"}, {"url": "http://www.homestosellmn.com/?paged=2", "positives": 1, "total": 67, "scan_date": "2018-07-26 14:17:53"}, {"url": "http://gatynes.com/", "positives": 1, "total": 67, "scan_date": "2018-07-26 14:07:50"}, {"url": "http://liversey.net/download/v20768?installer_file_name=Nicki+Minaj+-+Only+%28feat.+Drake%2C+Lil+Wayne+%26+Chris+Brown%29+%3D%26reffer%3Dhttp%3A%2F%2Fd.mrtzc.ch%2Fd_PKnuRP1.mp3%26product_name%3DNicki+Minaj+-+Only+%28feat.+Drake%2C+Lil+Wayne+%26product_title%3DNicki+Minaj", "positives": 2, "total": 67, "scan_date": "2018-07-26 13:48:43"}, {"url": "http://beerrecipes.bigtimberbrewingsupply.com/orange-ginger-sweet-mead/index.html", "positives": 3, "total": 67, "scan_date": "2018-07-26 13:40:28"}, {"url": "http://gestiondeempresas.org/wp-content/themes/wp-clear321/js/suckerfish.js", "positives": 3, "total": 67, "scan_date": "2018-07-26 12:52:01"}, {"url": "http://bzzeofbe.pornominer.com/t2278809b50.php", "positives": 1, "total": 67, "scan_date": "2018-07-26 12:46:33"}, {"url": "http://myaccount.id.apple.com.webapps-homesys39.goridesys.com/", "positives": 5, "total": 67, "scan_date": "2018-07-26 12:45:01"}, {"url": "http://beagle-care.com/index.html?p=174/", "positives": 2, "total": 67, "scan_date": "2018-07-26 12:24:32"}, {"url": "http://fortecegypt.com/blog/wp-content/themes/twentyfourteen/rrr.php?t=9f4ip23i3yu", "positives": 4, "total": 68, "scan_date": "2018-07-26 12:04:27"}, {"url": "http://www.cassahjlicia.com/MIys/Koras/", "positives": 6, "total": 67, "scan_date": "2018-07-26 12:02:15"}, {"url": "http://getyouryardsaleshere.com/data/sit/PAYPAL/Support-team/mpp/update_info/", "positives": 9, "total": 67, "scan_date": "2018-07-26 12:02:14"}, {"url": "http://dl.downloaddesktop3.info/1421011240/get7?", "positives": 1, "total": 67, "scan_date": "2018-07-26 11:51:17"}, {"url": "http://lmessage2readmywls.com/verify.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="General" numFmtId="164"/>
-  </numFmts>
-  <fonts count="4">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -434,34 +405,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+  <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -476,44 +432,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -540,14 +496,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -574,6 +548,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,189 +577,164 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B117"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C6" activeCellId="2" pane="topLeft" sqref="D2 D3 C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="2" width="14.16"/>
-    <col customWidth="1" max="2" min="2" style="2" width="11.05"/>
-    <col customWidth="1" max="1025" min="3" style="2" width="8.67"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="14.15625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="11.05078125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="3" spans="1:2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,721 +742,608 @@
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="2" s="3" spans="1:2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="3" s="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="4" s="3" spans="1:2">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="5" s="3" spans="1:2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="6" s="3" spans="1:2">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="7" s="3" spans="1:2">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="8" s="3" spans="1:2">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="9" s="3" spans="1:2">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="10" s="3" spans="1:2">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="11" s="3" spans="1:2">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="12" s="3" spans="1:2">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="13" s="3" spans="1:2">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="14" s="3" spans="1:2">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="15" s="3" spans="1:2">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="16" s="3" spans="1:2">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="17" s="3" spans="1:2">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="18" s="3" spans="1:2">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="19" s="3" spans="1:2">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="20" s="3" spans="1:2">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="21" s="3" spans="1:2">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="22" s="3" spans="1:2">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="23" s="3" spans="1:2">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="24" s="3" spans="1:2">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="25" s="3" spans="1:2">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="26" s="3" spans="1:2">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="27" s="3" spans="1:2">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="28" s="3" spans="1:2">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="29" s="3" spans="1:2">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="30" s="3" spans="1:2">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="31" s="3" spans="1:2">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="32" s="3" spans="1:2">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="33" s="3" spans="1:2">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="34" s="3" spans="1:2">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="35" s="3" spans="1:2">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="36" s="3" spans="1:2">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="37" s="3" spans="1:2">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="38" s="3" spans="1:2">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="39" s="3" spans="1:2">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="40" s="3" spans="1:2">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
         <v>42</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="41" s="3" spans="1:2">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="42" s="3" spans="1:2">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="43" s="3" spans="1:2">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
         <v>45</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="44" s="3" spans="1:2">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="45" s="3" spans="1:2">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="46" s="3" spans="1:2">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="47" s="3" spans="1:2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
         <v>49</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="48" s="3" spans="1:2">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="49" s="3" spans="1:2">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>51</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="50" s="3" spans="1:2">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="51" s="3" spans="1:2">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="52" s="3" spans="1:2">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>54</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="53" s="3" spans="1:2">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="54" s="3" spans="1:2">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>56</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="55" s="3" spans="1:2">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="56" s="3" spans="1:2">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="57" s="3" spans="1:2">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>59</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="58" s="3" spans="1:2">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>60</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="59" s="3" spans="1:2">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
         <v>61</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="60" s="3" spans="1:2">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="61" s="3" spans="1:2">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="62" s="3" spans="1:2">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>64</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="63" s="3" spans="1:2">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="64" s="3" spans="1:2">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="65" s="3" spans="1:2">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
         <v>67</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="66" s="3" spans="1:2">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
         <v>68</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="67" s="3" spans="1:2">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
         <v>69</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="68" s="3" spans="1:2">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
         <v>70</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="69" s="3" spans="1:2">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
         <v>71</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="70" s="3" spans="1:2">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="71" s="3" spans="1:2">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
         <v>73</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="72" s="3" spans="1:2">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>74</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="73" s="3" spans="1:2">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>75</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="74" s="3" spans="1:2">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
         <v>76</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="75" s="3" spans="1:2">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
         <v>77</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="76" s="3" spans="1:2">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
         <v>78</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="77" s="3" spans="1:2">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
         <v>79</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="78" s="3" spans="1:2">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="79" s="3" spans="1:2">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
         <v>81</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="80" s="3" spans="1:2">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
         <v>82</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="81" s="3" spans="1:2">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
         <v>83</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="82" s="3" spans="1:2">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
         <v>84</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="83" s="3" spans="1:2">
-      <c r="A83" s="2" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
         <v>85</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="84" s="3" spans="1:2">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
         <v>86</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="85" s="3" spans="1:2">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
         <v>87</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="86" s="3" spans="1:2">
-      <c r="A86" s="2" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
         <v>88</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="87" s="3" spans="1:2">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
         <v>89</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="88" s="3" spans="1:2">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
         <v>90</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="89" s="3" spans="1:2">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
         <v>91</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="90" s="3" spans="1:2">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
         <v>92</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="91" s="3" spans="1:2">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
         <v>93</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="92" s="3" spans="1:2">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
         <v>94</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="93" s="3" spans="1:2">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
         <v>95</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="94" s="3" spans="1:2">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
         <v>96</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="95" s="3" spans="1:2">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
         <v>97</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="96" s="3" spans="1:2">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
         <v>98</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="97" s="3" spans="1:2">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>99</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="98" s="3" spans="1:2">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
         <v>100</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="99" s="3" spans="1:2">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
         <v>101</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="100" s="3" spans="1:2">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
         <v>102</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="101" s="3" spans="1:2">
-      <c r="A101" s="2" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
         <v>103</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="102" s="3" spans="1:2">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
         <v>104</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="103" s="3" spans="1:2">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
         <v>105</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="104" s="3" spans="1:2">
-      <c r="A104" s="2" t="s">
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
         <v>106</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="105" s="3" spans="1:2">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
         <v>107</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="106" s="3" spans="1:2">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
         <v>108</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="107" s="3" spans="1:2">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
         <v>109</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="108" s="3" spans="1:2">
-      <c r="A108" s="2" t="s">
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
         <v>110</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="109" s="3" spans="1:2">
-      <c r="A109" s="2" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
         <v>111</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="110" s="3" spans="1:2">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
         <v>112</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="111" s="3" spans="1:2">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
         <v>113</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="112" s="3" spans="1:2">
-      <c r="A112" s="2" t="s">
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
         <v>114</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="113" s="3" spans="1:2">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
         <v>115</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="114" s="3" spans="1:2">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
         <v>116</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="115" s="3" spans="1:2">
-      <c r="A115" s="2" t="s">
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
         <v>117</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="116" s="3" spans="1:2">
-      <c r="A116" s="2" t="s">
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
         <v>118</v>
       </c>
     </row>
-    <row customHeight="1" ht="14.4" r="117" s="3" spans="1:2">
-      <c r="A117" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A2:D4"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D3" activeCellId="1" pane="topLeft" sqref="D2 D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row customHeight="1" ht="14.4" r="2" s="3" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="n"/>
-      <c r="D2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="14.4" r="3" s="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="n"/>
-      <c r="D3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4"/>
-  </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="2" pane="topLeft" sqref="D2 D3 A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-  <headerFooter differentFirst="0" differentOddEven="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="2" pane="topLeft" sqref="D2 D3 A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
-  <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="8.67"/>
-  </cols>
-  <sheetData/>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-  <headerFooter differentFirst="0" differentOddEven="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>